<commit_message>
Update Name of Algo
</commit_message>
<xml_diff>
--- a/data_impute_project/algorithm_result/terrestrial_mammals/combination_1_ABCD/A/10/seed1/result_data_KNN.xlsx
+++ b/data_impute_project/algorithm_result/terrestrial_mammals/combination_1_ABCD/A/10/seed1/result_data_KNN.xlsx
@@ -485,7 +485,7 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>-19.818</v>
+        <v>-20.218</v>
       </c>
       <c r="B4" t="n">
         <v>8.199999999999999</v>
@@ -527,7 +527,7 @@
     </row>
     <row r="7">
       <c r="A7" t="n">
-        <v>-20.20200000000001</v>
+        <v>-20.064</v>
       </c>
       <c r="B7" t="n">
         <v>9.43</v>
@@ -653,7 +653,7 @@
     </row>
     <row r="16">
       <c r="A16" t="n">
-        <v>-22.134</v>
+        <v>-22.119</v>
       </c>
       <c r="B16" t="n">
         <v>3.96</v>
@@ -821,7 +821,7 @@
     </row>
     <row r="28">
       <c r="A28" t="n">
-        <v>-21.814</v>
+        <v>-22.005</v>
       </c>
       <c r="B28" t="n">
         <v>5.47</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="29">
       <c r="A29" t="n">
-        <v>-21.042</v>
+        <v>-21.344</v>
       </c>
       <c r="B29" t="n">
         <v>7.52</v>
@@ -877,7 +877,7 @@
     </row>
     <row r="32">
       <c r="A32" t="n">
-        <v>-21.994</v>
+        <v>-21.782</v>
       </c>
       <c r="B32" t="n">
         <v>3.16</v>
@@ -989,7 +989,7 @@
     </row>
     <row r="40">
       <c r="A40" t="n">
-        <v>-19.7</v>
+        <v>-19.965</v>
       </c>
       <c r="B40" t="n">
         <v>10.75</v>
@@ -1157,7 +1157,7 @@
     </row>
     <row r="52">
       <c r="A52" t="n">
-        <v>-21.732</v>
+        <v>-21.957</v>
       </c>
       <c r="B52" t="n">
         <v>6.39</v>
@@ -1227,7 +1227,7 @@
     </row>
     <row r="57">
       <c r="A57" t="n">
-        <v>-22.214</v>
+        <v>-22.253</v>
       </c>
       <c r="B57" t="n">
         <v>4.82</v>
@@ -1353,7 +1353,7 @@
     </row>
     <row r="66">
       <c r="A66" t="n">
-        <v>-21.62</v>
+        <v>-21.53</v>
       </c>
       <c r="B66" t="n">
         <v>5.18</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="100">
       <c r="A100" t="n">
-        <v>-22.218</v>
+        <v>-22.352</v>
       </c>
       <c r="B100" t="n">
         <v>4.73</v>

</xml_diff>